<commit_message>
Update file with OEPS part numbers.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/pluma v.1.1 BOM.xlsx
+++ b/Hardware/PCB/pluma v.1.1 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Palma\Documents\GitHub\davidpalma666\pluma-main FORK\Hardware\PCB\pluma v.1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\emotional-cities\pluma\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBC2D45-CD9F-47D3-A9C3-BDADE67439DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7806D6A-D659-45BC-882A-26D070EBBD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmotionalCities BOM" sheetId="2" r:id="rId1"/>
@@ -19,10 +19,21 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'EmotionalCities BOM'!$A$4:$D$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="128">
   <si>
     <t>Designator</t>
   </si>
@@ -325,13 +336,109 @@
   </si>
   <si>
     <t>Pluma v.1.1 BOM</t>
+  </si>
+  <si>
+    <t>OEPS010004</t>
+  </si>
+  <si>
+    <t>OEPS010002</t>
+  </si>
+  <si>
+    <t>OEPS010017</t>
+  </si>
+  <si>
+    <t>OEPS010020</t>
+  </si>
+  <si>
+    <t>OEPS010011</t>
+  </si>
+  <si>
+    <t>OEPS010047</t>
+  </si>
+  <si>
+    <t>OEPS030010</t>
+  </si>
+  <si>
+    <t>OEPS080013</t>
+  </si>
+  <si>
+    <t>OEPS070015</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OEPS020001</t>
+  </si>
+  <si>
+    <t>OEPS020019</t>
+  </si>
+  <si>
+    <t>OEPS020041</t>
+  </si>
+  <si>
+    <t>OEPS020037</t>
+  </si>
+  <si>
+    <t>OEPS020030</t>
+  </si>
+  <si>
+    <t>OEPS020004</t>
+  </si>
+  <si>
+    <t>OEPS020083</t>
+  </si>
+  <si>
+    <t>OEPS080004</t>
+  </si>
+  <si>
+    <t>OEPS080012</t>
+  </si>
+  <si>
+    <t>OEPS080014</t>
+  </si>
+  <si>
+    <t>OEPS PN</t>
+  </si>
+  <si>
+    <t>OEPS080086</t>
+  </si>
+  <si>
+    <t>OEPS070071</t>
+  </si>
+  <si>
+    <t>OEPS070047</t>
+  </si>
+  <si>
+    <t>OEPS040003</t>
+  </si>
+  <si>
+    <t>OEPS100038</t>
+  </si>
+  <si>
+    <t>OEPS100039</t>
+  </si>
+  <si>
+    <t>OEPS100041</t>
+  </si>
+  <si>
+    <t>OEPS100040</t>
+  </si>
+  <si>
+    <t>To connect the boards use any standard header.</t>
+  </si>
+  <si>
+    <t>OEPS080087</t>
+  </si>
+  <si>
+    <t>OEPS070072</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +450,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,17 +481,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -397,6 +517,9 @@
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -412,12 +535,13 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{9AA3D3D8-4CFC-40EE-9E36-3A5FE2BEA9D4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="11">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="15" unboundColumnsRight="1">
+    <queryTableFields count="5">
       <queryTableField id="4" name="Quantity" tableColumnId="4"/>
       <queryTableField id="2" name="Designator" tableColumnId="2"/>
       <queryTableField id="5" name="Designation" tableColumnId="5"/>
       <queryTableField id="3" name="Footprint" tableColumnId="3"/>
+      <queryTableField id="11" dataBound="0" tableColumnId="1"/>
     </queryTableFields>
     <queryTableDeletedFields count="4">
       <deletedField name="Supplier and ref"/>
@@ -430,16 +554,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B18B008C-424A-4396-BBD4-772DB10D5BD9}" name="Table_EmotionalCities_BOM" displayName="Table_EmotionalCities_BOM" ref="A4:D39" tableType="queryTable" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A4:D39" xr:uid="{B18B008C-424A-4396-BBD4-772DB10D5BD9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B18B008C-424A-4396-BBD4-772DB10D5BD9}" name="Table_EmotionalCities_BOM" displayName="Table_EmotionalCities_BOM" ref="A4:E39" tableType="queryTable" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A4:E39" xr:uid="{B18B008C-424A-4396-BBD4-772DB10D5BD9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:D39">
     <sortCondition ref="B4:B39"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{04026F42-11BA-49E3-A590-A948F8CC75A9}" uniqueName="4" name="Quantity" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{6537FFB7-8DD1-4A99-B86C-FE9A469F7933}" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{CF7D2186-DFE8-41DD-A0A4-8690082C314D}" uniqueName="5" name="Designation" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{35ACC76B-226F-4973-9BF6-066573FDD75B}" uniqueName="3" name="Footprint" queryTableFieldId="3" dataDxfId="0"/>
+  <tableColumns count="5">
+    <tableColumn id="4" xr3:uid="{04026F42-11BA-49E3-A590-A948F8CC75A9}" uniqueName="4" name="Quantity" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6537FFB7-8DD1-4A99-B86C-FE9A469F7933}" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{CF7D2186-DFE8-41DD-A0A4-8690082C314D}" uniqueName="5" name="Designation" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{35ACC76B-226F-4973-9BF6-066573FDD75B}" uniqueName="3" name="Footprint" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C87AE3BC-3B38-4454-9CF7-FFD8744AB3B3}" uniqueName="1" name="OEPS PN" queryTableFieldId="11" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,44 +836,46 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D39"/>
+  <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="77.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>14</v>
       </c>
@@ -761,8 +888,11 @@
       <c r="D5" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -775,8 +905,11 @@
       <c r="D6" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -789,8 +922,11 @@
       <c r="D7" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -803,8 +939,9 @@
       <c r="D8" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -817,8 +954,11 @@
       <c r="D9" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -831,8 +971,11 @@
       <c r="D10" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -845,8 +988,11 @@
       <c r="D11" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -859,8 +1005,9 @@
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -873,8 +1020,11 @@
       <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -887,8 +1037,11 @@
       <c r="D14" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -901,8 +1054,11 @@
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -915,8 +1071,9 @@
       <c r="D16" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -929,8 +1086,11 @@
       <c r="D17" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -943,8 +1103,11 @@
       <c r="D18" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -957,8 +1120,11 @@
       <c r="D19" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -971,8 +1137,11 @@
       <c r="D20" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -985,8 +1154,11 @@
       <c r="D21" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>8</v>
       </c>
@@ -999,8 +1171,11 @@
       <c r="D22" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -1013,8 +1188,11 @@
       <c r="D23" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -1027,8 +1205,11 @@
       <c r="D24" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -1041,8 +1222,11 @@
       <c r="D25" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -1055,8 +1239,11 @@
       <c r="D26" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>8</v>
       </c>
@@ -1069,8 +1256,11 @@
       <c r="D27" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -1083,8 +1273,11 @@
       <c r="D28" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>4</v>
       </c>
@@ -1097,8 +1290,11 @@
       <c r="D29" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -1111,8 +1307,11 @@
       <c r="D30" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -1125,8 +1324,11 @@
       <c r="D31" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -1139,8 +1341,11 @@
       <c r="D32" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -1153,8 +1358,11 @@
       <c r="D33" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -1167,8 +1375,9 @@
       <c r="D34" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1</v>
       </c>
@@ -1181,8 +1390,11 @@
       <c r="D35" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -1195,8 +1407,11 @@
       <c r="D36" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E36" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -1209,8 +1424,11 @@
       <c r="D37" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -1223,8 +1441,11 @@
       <c r="D38" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -1237,10 +1458,19 @@
       <c r="D39" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="E39" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1253,7 +1483,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>